<commit_message>
Finish first draft of survey stuff
</commit_message>
<xml_diff>
--- a/Commit Validation.xlsx
+++ b/Commit Validation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Documents\University\General\UG4\SCC421\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D48A8E4-CE0E-4D8A-9531-38929E4F2C6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CDD336-AA2E-43EB-BA41-8164E8D0C81E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51416828-EB52-4DD8-85A1-39B47CECD07F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51416828-EB52-4DD8-85A1-39B47CECD07F}"/>
   </bookViews>
   <sheets>
     <sheet name="Commits" sheetId="2" r:id="rId1"/>
@@ -76,7 +76,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,13 +88,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -129,10 +122,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0857075-9E1B-49BB-AD0D-78B3E64BC41A}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,36 +511,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-    </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{477A147F-E227-4EF3-80D9-C429D77884F8}">
-      <formula1>"WinForms, Checkstyle, Signal-Server, NPM-CLI"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{E5E8D1A2-41EC-4720-AF67-362768A16744}">
-          <x14:formula1>
-            <xm:f>Options!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>D2:D15</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>